<commit_message>
Added a few tabs with different reference dates
</commit_message>
<xml_diff>
--- a/utils/tstart-tend.xlsx
+++ b/utils/tstart-tend.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leroquan\Documents\python\preprocessing-mitgcm\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC84D1C7-1B1C-4DA3-8626-444BE6AC6F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7F6DF-A2AD-4A4C-BE98-28306D061D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{1C1AAA8F-B7A7-4F2E-9366-9D04187454FC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{1C1AAA8F-B7A7-4F2E-9366-9D04187454FC}"/>
   </bookViews>
   <sheets>
     <sheet name="13.08.2023" sheetId="1" r:id="rId1"/>
-    <sheet name="01.12.2023" sheetId="2" r:id="rId2"/>
+    <sheet name="13.10.2023" sheetId="5" r:id="rId2"/>
+    <sheet name="01.05.2024" sheetId="6" r:id="rId3"/>
+    <sheet name="01.03.2024" sheetId="3" r:id="rId4"/>
+    <sheet name="01.12.2023" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="9">
   <si>
     <t xml:space="preserve">Tstart = </t>
   </si>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44742A8B-1D53-421F-BF8A-37CC7483A765}">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,6 +462,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1">
+        <f>C3</f>
         <v>4</v>
       </c>
     </row>
@@ -467,13 +471,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>4752000</v>
+        <v>668250</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
-        <v>45172</v>
+        <v>45170</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
@@ -491,19 +495,19 @@
       </c>
       <c r="I5" s="3">
         <f>G5-J5</f>
-        <v>45161</v>
+        <v>45163</v>
       </c>
       <c r="J5">
         <f>G4-G2</f>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>25650</v>
+      <c r="C6" s="1">
+        <v>668250</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
@@ -512,7 +516,7 @@
       </c>
       <c r="G8" s="1">
         <f>(G4-$G$2)*24*60*60</f>
-        <v>1814400</v>
+        <v>1641600</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
@@ -521,7 +525,7 @@
       </c>
       <c r="C9" s="2">
         <f>$C$2+C4/(24*60*60)</f>
-        <v>45206</v>
+        <v>45158.734375</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -546,7 +550,7 @@
       </c>
       <c r="G11">
         <f>G8/$G$3</f>
-        <v>453600</v>
+        <v>410400</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
@@ -554,9 +558,12 @@
         <v>6</v>
       </c>
       <c r="C12" s="3">
-        <f>$C$2+C6/(24*60*60)*4</f>
-        <v>45152.1875</v>
-      </c>
+        <f>$C$2+C6/(24*60*60)*C3</f>
+        <v>45181.9375</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -565,11 +572,302 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6008CE84-894C-451A-9E03-291ECF5C2511}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2139D2E-4F1E-4A61-856A-06D0CDD80A2A}">
+  <dimension ref="B2:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45212</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <f>C2</f>
+        <v>45212</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <f>C3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>668250</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45227</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7430400</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45238</v>
+      </c>
+      <c r="I5" s="3">
+        <f>G5-J5</f>
+        <v>45223</v>
+      </c>
+      <c r="J5">
+        <f>G4-G2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>581850</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(G4-$G$2)*24*60*60</f>
+        <v>1296000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$C$2+C4/(24*60*60)</f>
+        <v>45219.734375</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f>(G5-$G$2)*24*60*60</f>
+        <v>2246400</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <f>$C$2+C5/(24*60*60)</f>
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f>G8/$G$3</f>
+        <v>324000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <f>$C$2+C6/(24*60*60)*C3</f>
+        <v>45238.9375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC97997D-9312-494B-BC04-2DEDA6B4CBF2}">
+  <dimension ref="B2:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45389</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <f>C2</f>
+        <v>45389</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <f>C3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>668250</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45402</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7430400</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45414</v>
+      </c>
+      <c r="I5" s="3">
+        <f>G5-J5</f>
+        <v>45401</v>
+      </c>
+      <c r="J5">
+        <f>G4-G2</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>280800</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(G4-$G$2)*24*60*60</f>
+        <v>1123200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$C$2+C4/(24*60*60)</f>
+        <v>45396.734375</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f>(G5-$G$2)*24*60*60</f>
+        <v>2160000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <f>$C$2+C5/(24*60*60)</f>
+        <v>45475</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f>G8/$G$3</f>
+        <v>280800</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <f>$C$2+C6/(24*60*60)*C3</f>
+        <v>45402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A5D50E2-9360-4235-A4E1-0A171357575C}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,6 +884,147 @@
         <v>2</v>
       </c>
       <c r="C2" s="3">
+        <f>G2</f>
+        <v>45352</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <f>G3</f>
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4752000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45495.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>13996800</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45627</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3099600</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(G4-$G$2)*24*60*60</f>
+        <v>12398400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$C$2+C4/(24*60*60)</f>
+        <v>45407</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f>(G5-$G$2)*24*60*60</f>
+        <v>23760000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <f>$C$2+C5/(24*60*60)</f>
+        <v>45514</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f>G8/$G$3</f>
+        <v>3099600</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <f>$C$2+C6/(24*60*60)*$C$3</f>
+        <v>45495.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6008CE84-894C-451A-9E03-291ECF5C2511}">
+  <dimension ref="B2:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
         <v>45261</v>
       </c>
       <c r="F2" t="s">

</xml_diff>

<commit_message>
Can't be bothered to check everything I changed...
</commit_message>
<xml_diff>
--- a/utils/tstart-tend.xlsx
+++ b/utils/tstart-tend.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leroquan\Documents\python\preprocessing-mitgcm\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7F6DF-A2AD-4A4C-BE98-28306D061D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47616D3D-7FDE-425C-8B08-A8594F24E89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{1C1AAA8F-B7A7-4F2E-9366-9D04187454FC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="4" xr2:uid="{1C1AAA8F-B7A7-4F2E-9366-9D04187454FC}"/>
   </bookViews>
   <sheets>
     <sheet name="13.08.2023" sheetId="1" r:id="rId1"/>
     <sheet name="13.10.2023" sheetId="5" r:id="rId2"/>
     <sheet name="01.05.2024" sheetId="6" r:id="rId3"/>
     <sheet name="01.03.2024" sheetId="3" r:id="rId4"/>
-    <sheet name="01.12.2023" sheetId="2" r:id="rId5"/>
+    <sheet name="01.03.2025" sheetId="7" r:id="rId5"/>
+    <sheet name="01.12.2023" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
   <si>
     <t xml:space="preserve">Tstart = </t>
   </si>
@@ -866,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A5D50E2-9360-4235-A4E1-0A171357575C}">
   <dimension ref="B2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -900,13 +901,13 @@
       </c>
       <c r="C3" s="1">
         <f>G3</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
@@ -920,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="3">
-        <v>45495.5</v>
+        <v>45512</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
@@ -934,7 +935,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="3">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -943,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>3099600</v>
+        <v>432000</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
@@ -952,7 +953,7 @@
       </c>
       <c r="G8" s="1">
         <f>(G4-$G$2)*24*60*60</f>
-        <v>12398400</v>
+        <v>13824000</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
@@ -968,7 +969,7 @@
       </c>
       <c r="G9" s="1">
         <f>(G5-$G$2)*24*60*60</f>
-        <v>23760000</v>
+        <v>26438400</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
@@ -986,7 +987,7 @@
       </c>
       <c r="G11">
         <f>G8/$G$3</f>
-        <v>3099600</v>
+        <v>432000</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
@@ -995,7 +996,7 @@
       </c>
       <c r="C12" s="3">
         <f>$C$2+C6/(24*60*60)*$C$3</f>
-        <v>45495.5</v>
+        <v>45512</v>
       </c>
     </row>
   </sheetData>
@@ -1004,11 +1005,150 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A51DF43-86EE-492E-A53A-07CA1A9D5DFA}">
+  <dimension ref="B2:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <f>G2</f>
+        <v>45778</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <f>G3</f>
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4752000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45172</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7430400</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>396900</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(G4-$G$2)*24*60*60</f>
+        <v>-52358400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$C$2+C4/(24*60*60)</f>
+        <v>45833</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <f>(G5-$G$2)*24*60*60</f>
+        <v>-51494400</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <f>$C$2+C5/(24*60*60)</f>
+        <v>45864</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f>G8/$G$3</f>
+        <v>-1636200</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <f>$C$2+C6/(24*60*60)*4</f>
+        <v>45796.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6008CE84-894C-451A-9E03-291ECF5C2511}">
   <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>